<commit_message>
Update for Taiwan CDC data release on 20231024
</commit_message>
<xml_diff>
--- a/Taiwan-COVID19-data-2023.xlsx
+++ b/Taiwan-COVID19-data-2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chasenelson/scripts_NGS/github_Taiwan-COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF2C2B2-D153-584F-8A62-7E3C929D14A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119165F0-39E5-EB4E-8833-D25B8C8AAA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{836FDAF7-E370-6E4C-85E6-CE82AA0CAB02}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="113">
   <si>
     <t>NA</t>
   </si>
@@ -143,9 +143,6 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/WcWHyfVbjF05aooxyeUsQw?typeid=9</t>
   </si>
   <si>
-    <t>"Higher than"; "slowly increased from a low point"</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -360,6 +357,24 @@
   </si>
   <si>
     <t>Two days are missing; estimated as the mean of the previous (8/13-8/19) and following (8/22-8/28) periods</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-tfJGkCFKt8Lw21mY7G3Vw?typeid=9</t>
+  </si>
+  <si>
+    <t>Taiwan CDC changed its reporting the next week (source 2); new_deaths initially inferred to be 42 by the multiplication method but was reported explicitly as 44 in source 2</t>
+  </si>
+  <si>
+    <t>reporting_method_change</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Taiwan CDC changed its reporting, evidently in response to this repository posting on 20231023; new_deaths is now reported explicitly; DATES are not given</t>
   </si>
 </sst>
 </file>
@@ -369,7 +384,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -438,6 +453,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -484,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -502,6 +525,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -822,111 +848,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4771C105-BA87-EE45-8165-DB3BB9CF7A30}">
-  <dimension ref="A1:X37"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5" customWidth="1"/>
-    <col min="12" max="12" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="20" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="72.83203125" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="20" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.83203125" customWidth="1"/>
+    <col min="24" max="24" width="15.83203125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="72.83203125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>44980</v>
       </c>
@@ -937,73 +969,76 @@
         <v>44980</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D37" si="0">B2-A2+1</f>
+        <f t="shared" ref="D2:D38" si="0">B2-A2+1</f>
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>14387</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>9985320</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J37" si="1">H2</f>
+      <c r="J2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K37" si="1">I2</f>
         <v>9985320</v>
       </c>
-      <c r="K2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>37</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>19</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>18</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>50</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>90</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>17709</v>
       </c>
-      <c r="S2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <f>R2</f>
+      <c r="T2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>S2</f>
         <v>17709</v>
       </c>
-      <c r="U2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>44981</v>
       </c>
@@ -1014,44 +1049,44 @@
         <v>44987</v>
       </c>
       <c r="D3" s="1">
-        <f>B3-A3+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E3" s="1">
-        <f>A3-B2-1</f>
-        <v>0</v>
-      </c>
-      <c r="F3">
+        <f t="shared" ref="E3:E38" si="2">A3-B2-1</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3">
         <v>12032</v>
       </c>
-      <c r="G3" s="8">
-        <f>F3*D3</f>
+      <c r="H3" s="8">
+        <f>G3*D3</f>
         <v>84224</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>10069539</v>
       </c>
-      <c r="I3">
-        <f>H2+G3</f>
+      <c r="J3">
+        <f>I2+H3</f>
         <v>10069544</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f t="shared" si="1"/>
         <v>10069539</v>
       </c>
-      <c r="K3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3">
         <v>43</v>
       </c>
-      <c r="M3" s="8">
-        <f>L3*D3</f>
+      <c r="N3" s="8">
+        <f t="shared" ref="N3:N36" si="3">M3*D3</f>
         <v>301</v>
       </c>
-      <c r="N3" t="s">
-        <v>0</v>
-      </c>
       <c r="O3" t="s">
         <v>0</v>
       </c>
@@ -1061,29 +1096,31 @@
       <c r="Q3" t="s">
         <v>0</v>
       </c>
-      <c r="R3">
+      <c r="R3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>18010</v>
       </c>
-      <c r="S3">
-        <f>R2+M3</f>
+      <c r="T3">
+        <f>S2+N3</f>
         <v>18010</v>
       </c>
-      <c r="T3">
-        <f>R3</f>
+      <c r="U3">
+        <f>S3</f>
         <v>18010</v>
       </c>
-      <c r="U3" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="X3" s="11"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X3" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>44988</v>
       </c>
@@ -1098,40 +1135,40 @@
         <v>7</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E37" si="2">A4-B3-1</f>
-        <v>0</v>
-      </c>
-      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4">
         <v>10609</v>
       </c>
-      <c r="G4" s="8">
-        <f>F4*D4</f>
+      <c r="H4" s="8">
+        <f>G4*D4</f>
         <v>74263</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>10143788</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I5" si="3">H3+G4</f>
+      <c r="J4">
+        <f t="shared" ref="J4:J5" si="4">I3+H4</f>
         <v>10143802</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="1"/>
         <v>10143788</v>
       </c>
-      <c r="K4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4">
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4">
         <v>52</v>
       </c>
-      <c r="M4" s="8">
-        <f t="shared" ref="M4:M37" si="4">L4*D4</f>
+      <c r="N4" s="8">
+        <f t="shared" si="3"/>
         <v>364</v>
       </c>
-      <c r="N4" t="s">
-        <v>0</v>
-      </c>
       <c r="O4" t="s">
         <v>0</v>
       </c>
@@ -1141,29 +1178,31 @@
       <c r="Q4" t="s">
         <v>0</v>
       </c>
-      <c r="R4">
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>18371</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S5" si="5">R3+M4</f>
+      <c r="T4">
+        <f t="shared" ref="T4:T5" si="5">S3+N4</f>
         <v>18374</v>
       </c>
-      <c r="T4">
-        <f>R4</f>
+      <c r="U4">
+        <f>S4</f>
         <v>18371</v>
       </c>
-      <c r="U4" t="s">
-        <v>55</v>
-      </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" t="s">
+        <v>54</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="X4" s="11"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X4" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>44995</v>
       </c>
@@ -1181,37 +1220,37 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5">
         <v>8959</v>
       </c>
-      <c r="G5" s="8">
-        <f>F5*D5</f>
+      <c r="H5" s="8">
+        <f>G5*D5</f>
         <v>62713</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>10206482</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="3"/>
+      <c r="J5">
+        <f t="shared" si="4"/>
         <v>10206501</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>10206482</v>
       </c>
-      <c r="K5" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5">
+      <c r="L5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5">
         <v>41</v>
       </c>
-      <c r="M5" s="8">
-        <f t="shared" si="4"/>
+      <c r="N5" s="8">
+        <f t="shared" si="3"/>
         <v>287</v>
       </c>
-      <c r="N5" t="s">
-        <v>0</v>
-      </c>
       <c r="O5" t="s">
         <v>0</v>
       </c>
@@ -1221,29 +1260,31 @@
       <c r="Q5" t="s">
         <v>0</v>
       </c>
-      <c r="R5">
+      <c r="R5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>18656</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <f t="shared" si="5"/>
         <v>18658</v>
       </c>
-      <c r="T5">
-        <f>R5</f>
+      <c r="U5">
+        <f>S5</f>
         <v>18656</v>
       </c>
-      <c r="U5" t="s">
-        <v>58</v>
-      </c>
-      <c r="V5" s="3" t="s">
+      <c r="V5" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X5" s="11"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>45002</v>
       </c>
@@ -1261,56 +1302,59 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="F6" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
       </c>
-      <c r="J6" t="str">
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6">
+      <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6">
         <v>34</v>
       </c>
-      <c r="M6" s="8">
-        <f t="shared" si="4"/>
+      <c r="N6" s="8">
+        <f t="shared" si="3"/>
         <v>238</v>
       </c>
-      <c r="R6" t="s">
-        <v>0</v>
-      </c>
       <c r="S6" t="s">
         <v>0</v>
       </c>
-      <c r="T6" s="8">
-        <f>T5+M6</f>
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="8">
+        <f>U5+N6</f>
         <v>18894</v>
       </c>
-      <c r="U6" t="s">
-        <v>60</v>
-      </c>
-      <c r="V6" s="3" t="s">
+      <c r="V6" t="s">
+        <v>59</v>
+      </c>
+      <c r="W6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="X6" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>45009</v>
       </c>
@@ -1328,54 +1372,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="F7" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" t="str">
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L7">
+      <c r="L7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7">
         <v>25</v>
       </c>
-      <c r="M7" s="8">
-        <f t="shared" si="4"/>
+      <c r="N7" s="8">
+        <f t="shared" si="3"/>
         <v>175</v>
       </c>
-      <c r="R7" t="s">
-        <v>0</v>
-      </c>
       <c r="S7" t="s">
         <v>0</v>
       </c>
-      <c r="T7" s="8">
-        <f t="shared" ref="T7:T22" si="6">T6+M7</f>
+      <c r="T7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" s="8">
+        <f t="shared" ref="U7:U22" si="6">U6+N7</f>
         <v>19069</v>
       </c>
-      <c r="U7" t="s">
-        <v>60</v>
-      </c>
-      <c r="V7" s="3" t="s">
+      <c r="V7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="X7" s="11"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>45016</v>
       </c>
@@ -1393,54 +1439,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="F8" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="J8" t="str">
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8">
+      <c r="L8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8">
         <v>15</v>
       </c>
-      <c r="M8" s="8">
-        <f t="shared" si="4"/>
+      <c r="N8" s="8">
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="R8" t="s">
-        <v>0</v>
-      </c>
       <c r="S8" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="8">
+      <c r="T8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U8" s="8">
         <f t="shared" si="6"/>
         <v>19189</v>
       </c>
-      <c r="U8" t="s">
-        <v>60</v>
-      </c>
-      <c r="V8" s="3" t="s">
+      <c r="V8" t="s">
+        <v>59</v>
+      </c>
+      <c r="W8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="W8" s="3" t="s">
+      <c r="X8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="X8" s="11"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>45024</v>
       </c>
@@ -1458,54 +1506,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="F9" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="J9" t="str">
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K9" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9">
+      <c r="L9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9">
         <v>17</v>
       </c>
-      <c r="M9" s="8">
-        <f t="shared" si="4"/>
+      <c r="N9" s="8">
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
-      <c r="R9" t="s">
-        <v>0</v>
-      </c>
       <c r="S9" t="s">
         <v>0</v>
       </c>
-      <c r="T9" s="8">
+      <c r="T9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" s="8">
         <f t="shared" si="6"/>
         <v>19291</v>
       </c>
-      <c r="U9" t="s">
-        <v>66</v>
-      </c>
-      <c r="V9" s="3" t="s">
+      <c r="V9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="W9" s="3" t="s">
+      <c r="X9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="X9" s="11"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>45030</v>
       </c>
@@ -1523,56 +1573,59 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F10" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I10" t="s">
         <v>0</v>
       </c>
-      <c r="J10" t="str">
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K10" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10">
+      <c r="L10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10">
         <v>13</v>
       </c>
-      <c r="M10" s="8">
-        <f t="shared" si="4"/>
+      <c r="N10" s="8">
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="R10" t="s">
-        <v>0</v>
-      </c>
       <c r="S10" t="s">
         <v>0</v>
       </c>
-      <c r="T10" s="8">
+      <c r="T10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U10" s="8">
         <f t="shared" si="6"/>
         <v>19382</v>
       </c>
-      <c r="U10" t="s">
-        <v>67</v>
-      </c>
-      <c r="V10" s="3" t="s">
+      <c r="V10" t="s">
+        <v>66</v>
+      </c>
+      <c r="W10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>45037</v>
       </c>
@@ -1591,56 +1644,59 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="F11" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I11" t="s">
         <v>0</v>
       </c>
-      <c r="J11" t="str">
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" s="11">
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="11">
         <v>13</v>
       </c>
-      <c r="M11" s="8">
-        <f t="shared" si="4"/>
+      <c r="N11" s="8">
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="R11" t="s">
-        <v>0</v>
-      </c>
       <c r="S11" t="s">
         <v>0</v>
       </c>
-      <c r="T11" s="8">
+      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="8">
         <f t="shared" si="6"/>
         <v>19473</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
+        <v>69</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X11" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="V11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y11" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>45044</v>
       </c>
@@ -1658,56 +1714,59 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F12" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I12" t="s">
         <v>0</v>
       </c>
-      <c r="J12" t="str">
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K12" t="s">
-        <v>72</v>
-      </c>
-      <c r="L12">
+      <c r="L12" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12">
         <v>12</v>
       </c>
-      <c r="M12" s="8">
-        <f t="shared" si="4"/>
+      <c r="N12" s="8">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="R12" t="s">
-        <v>0</v>
-      </c>
       <c r="S12" t="s">
         <v>0</v>
       </c>
-      <c r="T12" s="8">
+      <c r="T12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" s="8">
         <f t="shared" si="6"/>
         <v>19497</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
+        <v>69</v>
+      </c>
+      <c r="W12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="V12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="W12" s="3" t="s">
+      <c r="X12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="X12" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y12" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>45046</v>
       </c>
@@ -1725,54 +1784,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F13" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="F13" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>0</v>
       </c>
-      <c r="J13" t="str">
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K13" t="s">
-        <v>72</v>
-      </c>
-      <c r="L13">
+      <c r="L13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13">
         <v>15</v>
       </c>
-      <c r="M13" s="8">
-        <f t="shared" si="4"/>
+      <c r="N13" s="8">
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="R13" t="s">
-        <v>0</v>
-      </c>
       <c r="S13" t="s">
         <v>0</v>
       </c>
-      <c r="T13" s="8">
+      <c r="T13" t="s">
+        <v>0</v>
+      </c>
+      <c r="U13" s="8">
         <f t="shared" si="6"/>
         <v>19602</v>
       </c>
-      <c r="U13" t="s">
-        <v>72</v>
-      </c>
-      <c r="V13" s="3" t="s">
+      <c r="V13" t="s">
+        <v>71</v>
+      </c>
+      <c r="W13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="W13" s="3" t="s">
+      <c r="X13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X13" s="11"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>45053</v>
       </c>
@@ -1790,54 +1851,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="F14" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I14" t="s">
         <v>0</v>
       </c>
-      <c r="J14" t="str">
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K14" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14">
+      <c r="L14" t="s">
+        <v>74</v>
+      </c>
+      <c r="M14">
         <v>15</v>
       </c>
-      <c r="M14" s="8">
-        <f t="shared" si="4"/>
+      <c r="N14" s="8">
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="R14" t="s">
-        <v>0</v>
-      </c>
       <c r="S14" t="s">
         <v>0</v>
       </c>
-      <c r="T14" s="8">
+      <c r="T14" t="s">
+        <v>0</v>
+      </c>
+      <c r="U14" s="8">
         <f t="shared" si="6"/>
         <v>19707</v>
       </c>
-      <c r="U14" t="s">
-        <v>70</v>
-      </c>
-      <c r="V14" s="3" t="s">
+      <c r="V14" t="s">
+        <v>69</v>
+      </c>
+      <c r="W14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="X14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="X14" s="11"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>45060</v>
       </c>
@@ -1855,54 +1918,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="F15" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I15" t="s">
         <v>0</v>
       </c>
-      <c r="J15" t="str">
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K15" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15">
+      <c r="L15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15">
         <v>18</v>
       </c>
-      <c r="M15" s="8">
-        <f t="shared" si="4"/>
+      <c r="N15" s="8">
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="R15" t="s">
-        <v>0</v>
-      </c>
       <c r="S15" t="s">
         <v>0</v>
       </c>
-      <c r="T15" s="8">
+      <c r="T15" t="s">
+        <v>0</v>
+      </c>
+      <c r="U15" s="8">
         <f t="shared" si="6"/>
         <v>19833</v>
       </c>
-      <c r="U15" t="s">
-        <v>75</v>
-      </c>
-      <c r="V15" s="3" t="s">
+      <c r="V15" t="s">
+        <v>74</v>
+      </c>
+      <c r="W15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="W15" s="3" t="s">
+      <c r="X15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="X15" s="11"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>45067</v>
       </c>
@@ -1920,54 +1985,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="F16" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I16" t="s">
         <v>0</v>
       </c>
-      <c r="J16" t="str">
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K16" t="s">
-        <v>75</v>
-      </c>
-      <c r="L16">
+      <c r="L16" t="s">
+        <v>74</v>
+      </c>
+      <c r="M16">
         <v>20</v>
       </c>
-      <c r="M16" s="8">
-        <f t="shared" si="4"/>
+      <c r="N16" s="8">
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="R16" t="s">
-        <v>0</v>
-      </c>
       <c r="S16" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="8">
+      <c r="T16" t="s">
+        <v>0</v>
+      </c>
+      <c r="U16" s="8">
         <f t="shared" si="6"/>
         <v>19973</v>
       </c>
-      <c r="U16" t="s">
-        <v>75</v>
-      </c>
-      <c r="V16" s="3" t="s">
+      <c r="V16" t="s">
+        <v>74</v>
+      </c>
+      <c r="W16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="W16" s="3" t="s">
+      <c r="X16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="X16" s="11"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>45074</v>
       </c>
@@ -1985,54 +2052,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="F17" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I17" t="s">
         <v>0</v>
       </c>
-      <c r="J17" t="str">
+      <c r="J17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K17" t="s">
-        <v>76</v>
-      </c>
-      <c r="L17">
+      <c r="L17" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17">
         <v>28</v>
       </c>
-      <c r="M17" s="8">
-        <f t="shared" si="4"/>
+      <c r="N17" s="8">
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
-      <c r="R17" t="s">
-        <v>0</v>
-      </c>
       <c r="S17" t="s">
         <v>0</v>
       </c>
-      <c r="T17" s="8">
+      <c r="T17" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="8">
         <f t="shared" si="6"/>
         <v>20169</v>
       </c>
-      <c r="U17" t="s">
-        <v>75</v>
-      </c>
-      <c r="V17" s="3" t="s">
+      <c r="V17" t="s">
+        <v>74</v>
+      </c>
+      <c r="W17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W17" s="3" t="s">
+      <c r="X17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="X17" s="11"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>45081</v>
       </c>
@@ -2050,54 +2119,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="F18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>0</v>
       </c>
-      <c r="J18" t="str">
+      <c r="J18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K18" t="s">
-        <v>77</v>
-      </c>
-      <c r="L18">
+      <c r="L18" t="s">
+        <v>76</v>
+      </c>
+      <c r="M18">
         <v>35</v>
       </c>
-      <c r="M18" s="8">
-        <f t="shared" si="4"/>
+      <c r="N18" s="8">
+        <f t="shared" si="3"/>
         <v>245</v>
       </c>
-      <c r="R18" t="s">
-        <v>0</v>
-      </c>
       <c r="S18" t="s">
         <v>0</v>
       </c>
-      <c r="T18" s="8">
+      <c r="T18" t="s">
+        <v>0</v>
+      </c>
+      <c r="U18" s="8">
         <f t="shared" si="6"/>
         <v>20414</v>
       </c>
-      <c r="U18" t="s">
-        <v>64</v>
-      </c>
-      <c r="V18" s="3" t="s">
+      <c r="V18" t="s">
+        <v>63</v>
+      </c>
+      <c r="W18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="X18" s="11"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X18" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>45088</v>
       </c>
@@ -2115,54 +2186,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="F19" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I19" t="s">
         <v>0</v>
       </c>
-      <c r="J19" t="str">
+      <c r="J19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K19" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19">
+      <c r="L19" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19">
         <v>30</v>
       </c>
-      <c r="M19" s="8">
-        <f t="shared" si="4"/>
+      <c r="N19" s="8">
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
-      <c r="R19" t="s">
-        <v>0</v>
-      </c>
       <c r="S19" t="s">
         <v>0</v>
       </c>
-      <c r="T19" s="8">
+      <c r="T19" t="s">
+        <v>0</v>
+      </c>
+      <c r="U19" s="8">
         <f t="shared" si="6"/>
         <v>20624</v>
       </c>
-      <c r="U19" t="s">
-        <v>79</v>
-      </c>
-      <c r="V19" s="3" t="s">
+      <c r="V19" t="s">
         <v>78</v>
       </c>
       <c r="W19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="X19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="X19" s="11"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <v>45095</v>
       </c>
@@ -2180,56 +2253,59 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F20" t="s">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="F20" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I20" t="s">
         <v>0</v>
       </c>
-      <c r="J20" t="str">
+      <c r="J20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K20" t="s">
-        <v>82</v>
-      </c>
-      <c r="L20">
+      <c r="L20" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20">
         <v>24</v>
       </c>
-      <c r="M20" s="8">
-        <f t="shared" si="4"/>
+      <c r="N20" s="8">
+        <f t="shared" si="3"/>
         <v>168</v>
       </c>
-      <c r="R20" t="s">
-        <v>0</v>
-      </c>
       <c r="S20" t="s">
         <v>0</v>
       </c>
-      <c r="T20" s="8">
+      <c r="T20" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" s="8">
         <f t="shared" si="6"/>
         <v>20792</v>
       </c>
-      <c r="U20" t="s">
-        <v>81</v>
-      </c>
-      <c r="V20" s="3" t="s">
+      <c r="V20" t="s">
+        <v>80</v>
+      </c>
+      <c r="W20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W20" s="3" t="s">
+      <c r="X20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="X20" s="11" t="s">
+      <c r="Y20" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <v>45102</v>
       </c>
@@ -2247,56 +2323,59 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="F21" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I21" t="s">
         <v>0</v>
       </c>
-      <c r="J21" t="str">
+      <c r="J21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K21" t="s">
-        <v>84</v>
-      </c>
-      <c r="L21">
+      <c r="L21" t="s">
+        <v>83</v>
+      </c>
+      <c r="M21">
         <v>45</v>
       </c>
-      <c r="M21" s="8">
-        <f t="shared" si="4"/>
+      <c r="N21" s="8">
+        <f t="shared" si="3"/>
         <v>315</v>
       </c>
-      <c r="R21" t="s">
-        <v>0</v>
-      </c>
       <c r="S21" t="s">
         <v>0</v>
       </c>
-      <c r="T21" s="8">
+      <c r="T21" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" s="8">
         <f t="shared" si="6"/>
         <v>21107</v>
       </c>
-      <c r="U21" t="s">
-        <v>64</v>
-      </c>
-      <c r="V21" s="3" t="s">
+      <c r="V21" t="s">
+        <v>63</v>
+      </c>
+      <c r="W21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="W21" s="3" t="s">
+      <c r="X21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X21" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y21" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <v>45109</v>
       </c>
@@ -2314,54 +2393,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F22" t="s">
-        <v>0</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="F22" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I22" t="s">
         <v>0</v>
       </c>
-      <c r="J22" t="str">
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K22" t="s">
-        <v>86</v>
-      </c>
-      <c r="L22">
+      <c r="L22" t="s">
+        <v>85</v>
+      </c>
+      <c r="M22">
         <v>33</v>
       </c>
-      <c r="M22" s="8">
-        <f t="shared" si="4"/>
+      <c r="N22" s="8">
+        <f t="shared" si="3"/>
         <v>231</v>
       </c>
-      <c r="R22" t="s">
-        <v>0</v>
-      </c>
       <c r="S22" t="s">
         <v>0</v>
       </c>
-      <c r="T22" s="8">
+      <c r="T22" t="s">
+        <v>0</v>
+      </c>
+      <c r="U22" s="8">
         <f t="shared" si="6"/>
         <v>21338</v>
       </c>
-      <c r="U22" t="s">
-        <v>85</v>
-      </c>
-      <c r="V22" s="3" t="s">
+      <c r="V22" t="s">
+        <v>84</v>
+      </c>
+      <c r="W22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W22" s="3" t="s">
+      <c r="X22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X22" s="11"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>45116</v>
       </c>
@@ -2379,54 +2460,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="F23" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I23" t="s">
         <v>0</v>
       </c>
-      <c r="J23" t="str">
+      <c r="J23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K23" t="s">
-        <v>88</v>
-      </c>
-      <c r="L23">
+      <c r="L23" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23">
         <v>36</v>
       </c>
-      <c r="M23" s="8">
-        <f t="shared" si="4"/>
+      <c r="N23" s="8">
+        <f t="shared" si="3"/>
         <v>252</v>
       </c>
-      <c r="R23" t="s">
-        <v>0</v>
-      </c>
       <c r="S23" t="s">
         <v>0</v>
       </c>
-      <c r="T23" s="8">
-        <f>T22+M23</f>
+      <c r="T23" t="s">
+        <v>0</v>
+      </c>
+      <c r="U23" s="8">
+        <f>U22+N23</f>
         <v>21590</v>
       </c>
-      <c r="U23" t="s">
-        <v>87</v>
-      </c>
-      <c r="V23" s="3" t="s">
+      <c r="V23" t="s">
+        <v>86</v>
+      </c>
+      <c r="W23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W23" s="3" t="s">
+      <c r="X23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X23" s="11"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>45123</v>
       </c>
@@ -2444,54 +2527,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="F24" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I24" t="s">
         <v>0</v>
       </c>
-      <c r="J24" t="str">
+      <c r="J24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K24" t="s">
-        <v>90</v>
-      </c>
-      <c r="L24">
+      <c r="L24" t="s">
+        <v>89</v>
+      </c>
+      <c r="M24">
         <v>28</v>
       </c>
-      <c r="M24" s="8">
-        <f t="shared" si="4"/>
+      <c r="N24" s="8">
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
-      <c r="R24" t="s">
-        <v>0</v>
-      </c>
       <c r="S24" t="s">
         <v>0</v>
       </c>
-      <c r="T24" s="8">
-        <f t="shared" ref="T24:T37" si="7">T23+M24</f>
+      <c r="T24" t="s">
+        <v>0</v>
+      </c>
+      <c r="U24" s="8">
+        <f t="shared" ref="U24:U36" si="7">U23+N24</f>
         <v>21786</v>
       </c>
-      <c r="U24" t="s">
-        <v>89</v>
-      </c>
-      <c r="V24" s="3" t="s">
+      <c r="V24" t="s">
+        <v>88</v>
+      </c>
+      <c r="W24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W24" s="3" t="s">
+      <c r="X24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X24" s="11"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <v>45130</v>
       </c>
@@ -2509,54 +2594,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="F25" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I25" t="s">
         <v>0</v>
       </c>
-      <c r="J25" t="str">
+      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K25" t="s">
-        <v>92</v>
-      </c>
-      <c r="L25">
+      <c r="L25" t="s">
+        <v>91</v>
+      </c>
+      <c r="M25">
         <v>25</v>
       </c>
-      <c r="M25" s="8">
-        <f t="shared" si="4"/>
+      <c r="N25" s="8">
+        <f t="shared" si="3"/>
         <v>175</v>
       </c>
-      <c r="R25" t="s">
-        <v>0</v>
-      </c>
       <c r="S25" t="s">
         <v>0</v>
       </c>
-      <c r="T25" s="8">
+      <c r="T25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U25" s="8">
         <f t="shared" si="7"/>
         <v>21961</v>
       </c>
-      <c r="U25" t="s">
-        <v>91</v>
-      </c>
-      <c r="V25" s="3" t="s">
+      <c r="V25" t="s">
+        <v>90</v>
+      </c>
+      <c r="W25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="W25" s="3" t="s">
+      <c r="X25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X25" s="11"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>45137</v>
       </c>
@@ -2574,54 +2661,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="F26" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I26" t="s">
         <v>0</v>
       </c>
-      <c r="J26" t="str">
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K26" t="s">
-        <v>94</v>
-      </c>
-      <c r="L26">
+      <c r="L26" t="s">
+        <v>93</v>
+      </c>
+      <c r="M26">
         <v>18</v>
       </c>
-      <c r="M26" s="8">
-        <f t="shared" si="4"/>
+      <c r="N26" s="8">
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="R26" t="s">
-        <v>0</v>
-      </c>
       <c r="S26" t="s">
         <v>0</v>
       </c>
-      <c r="T26" s="8">
+      <c r="T26" t="s">
+        <v>0</v>
+      </c>
+      <c r="U26" s="8">
         <f t="shared" si="7"/>
         <v>22087</v>
       </c>
-      <c r="U26" t="s">
-        <v>93</v>
-      </c>
-      <c r="V26" s="3" t="s">
+      <c r="V26" t="s">
+        <v>92</v>
+      </c>
+      <c r="W26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W26" s="3" t="s">
+      <c r="X26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X26" s="11"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>45144</v>
       </c>
@@ -2639,70 +2728,72 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="F27" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I27" t="s">
         <v>0</v>
       </c>
-      <c r="J27" t="str">
+      <c r="J27" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L27">
+      <c r="L27" t="s">
+        <v>94</v>
+      </c>
+      <c r="M27">
         <v>14</v>
       </c>
-      <c r="M27" s="8">
-        <f t="shared" si="4"/>
+      <c r="N27" s="8">
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
-      <c r="N27" s="8">
-        <f t="shared" ref="N27:N28" si="8">M27*E27</f>
-        <v>0</v>
-      </c>
-      <c r="O27" s="8" t="e">
-        <f t="shared" ref="O27:O28" si="9">N27*F27</f>
+      <c r="O27" s="8">
+        <f t="shared" ref="O27:O28" si="8">N27*E27</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="8" t="e">
+        <f t="shared" ref="P27:P28" si="9">O27*G27</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P27" s="8" t="e">
-        <f t="shared" ref="P27:P28" si="10">O27*G27</f>
+      <c r="Q27" s="8" t="e">
+        <f t="shared" ref="Q27:Q28" si="10">P27*H27</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q27" s="8" t="e">
-        <f t="shared" ref="Q27:Q28" si="11">P27*H27</f>
+      <c r="R27" s="8" t="e">
+        <f t="shared" ref="R27:R28" si="11">Q27*I27</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R27" t="s">
-        <v>0</v>
-      </c>
       <c r="S27" t="s">
         <v>0</v>
       </c>
-      <c r="T27" s="8">
+      <c r="T27" t="s">
+        <v>0</v>
+      </c>
+      <c r="U27" s="8">
         <f t="shared" si="7"/>
         <v>22185</v>
       </c>
-      <c r="U27" t="s">
-        <v>89</v>
-      </c>
-      <c r="V27" s="3" t="s">
+      <c r="V27" t="s">
+        <v>88</v>
+      </c>
+      <c r="W27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="W27" s="3" t="s">
+      <c r="X27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="X27" s="11"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>45151</v>
       </c>
@@ -2720,70 +2811,72 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F28" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="F28" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I28" t="s">
         <v>0</v>
       </c>
-      <c r="J28" t="str">
+      <c r="J28" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K28" t="s">
-        <v>97</v>
-      </c>
-      <c r="L28">
+      <c r="L28" t="s">
+        <v>96</v>
+      </c>
+      <c r="M28">
         <v>11</v>
       </c>
-      <c r="M28" s="8">
-        <f>L28*D28</f>
+      <c r="N28" s="8">
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
-      <c r="N28" s="8">
+      <c r="O28" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O28" s="8" t="e">
+      <c r="P28" s="8" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="P28" s="8" t="e">
+      <c r="Q28" s="8" t="e">
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q28" s="8" t="e">
+      <c r="R28" s="8" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="R28" t="s">
-        <v>0</v>
-      </c>
       <c r="S28" t="s">
         <v>0</v>
       </c>
-      <c r="T28" s="8">
+      <c r="T28" t="s">
+        <v>0</v>
+      </c>
+      <c r="U28" s="8">
         <f t="shared" si="7"/>
         <v>22262</v>
       </c>
-      <c r="U28" t="s">
-        <v>96</v>
-      </c>
-      <c r="V28" s="3" t="s">
+      <c r="V28" t="s">
+        <v>95</v>
+      </c>
+      <c r="W28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W28" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="X28" s="11"/>
-    </row>
-    <row r="29" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X28" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
         <v>45158</v>
       </c>
@@ -2801,57 +2894,60 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="11" t="s">
+      <c r="F29" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="15" t="s">
         <v>0</v>
       </c>
       <c r="I29" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J29" s="11" t="str">
-        <f t="shared" ref="J29" si="12">H29</f>
+      <c r="J29" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" s="11" t="str">
+        <f t="shared" ref="K29" si="12">I29</f>
         <v>NA</v>
       </c>
-      <c r="K29" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L29" s="11">
-        <f>AVERAGE(L28,L30)</f>
+      <c r="L29" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="11">
+        <f>AVERAGE(M28,M30)</f>
         <v>13</v>
       </c>
-      <c r="M29" s="15">
-        <f t="shared" si="4"/>
+      <c r="N29" s="15">
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="R29" s="11" t="s">
-        <v>0</v>
-      </c>
       <c r="S29" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="T29" s="15">
+      <c r="T29" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U29" s="15">
         <f t="shared" si="7"/>
         <v>22288</v>
       </c>
-      <c r="U29" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V29" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="W29" s="11" t="s">
+      <c r="V29" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W29" s="16" t="s">
         <v>0</v>
       </c>
       <c r="X29" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>45160</v>
       </c>
@@ -2869,56 +2965,59 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F30" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="F30" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I30" t="s">
         <v>0</v>
       </c>
-      <c r="J30" t="str">
+      <c r="J30" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K30" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="L30">
+      <c r="L30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30">
         <v>15</v>
       </c>
-      <c r="M30" s="8">
-        <f t="shared" si="4"/>
+      <c r="N30" s="8">
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="R30" t="s">
-        <v>0</v>
-      </c>
       <c r="S30" t="s">
         <v>0</v>
       </c>
-      <c r="T30" s="8">
+      <c r="T30" t="s">
+        <v>0</v>
+      </c>
+      <c r="U30" s="8">
         <f t="shared" si="7"/>
         <v>22393</v>
       </c>
-      <c r="U30" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="V30" s="3" t="s">
+      <c r="V30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="W30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="W30" s="3" t="s">
+      <c r="X30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X30" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y30" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <v>45167</v>
       </c>
@@ -2936,54 +3035,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="F31" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I31" t="s">
         <v>0</v>
       </c>
-      <c r="J31" t="str">
+      <c r="J31" t="s">
+        <v>0</v>
+      </c>
+      <c r="K31" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K31" t="s">
-        <v>77</v>
-      </c>
-      <c r="L31">
+      <c r="L31" t="s">
+        <v>76</v>
+      </c>
+      <c r="M31">
         <v>8</v>
       </c>
-      <c r="M31" s="8">
-        <f t="shared" si="4"/>
+      <c r="N31" s="8">
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="R31" t="s">
-        <v>0</v>
-      </c>
       <c r="S31" t="s">
         <v>0</v>
       </c>
-      <c r="T31" s="8">
+      <c r="T31" t="s">
+        <v>0</v>
+      </c>
+      <c r="U31" s="8">
         <f t="shared" si="7"/>
         <v>22449</v>
       </c>
-      <c r="U31" t="s">
-        <v>100</v>
-      </c>
-      <c r="V31" s="3" t="s">
+      <c r="V31" t="s">
+        <v>99</v>
+      </c>
+      <c r="W31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="W31" s="3" t="s">
+      <c r="X31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="X31" s="11"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>45174</v>
       </c>
@@ -3001,54 +3102,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="F32" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I32" t="s">
         <v>0</v>
       </c>
-      <c r="J32" t="str">
+      <c r="J32" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K32" t="s">
-        <v>64</v>
-      </c>
-      <c r="L32">
+      <c r="L32" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32">
         <v>6</v>
       </c>
-      <c r="M32" s="8">
-        <f t="shared" si="4"/>
+      <c r="N32" s="8">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="R32" t="s">
-        <v>0</v>
-      </c>
       <c r="S32" t="s">
         <v>0</v>
       </c>
-      <c r="T32" s="8">
+      <c r="T32" t="s">
+        <v>0</v>
+      </c>
+      <c r="U32" s="8">
         <f t="shared" si="7"/>
         <v>22491</v>
       </c>
-      <c r="U32" t="s">
-        <v>60</v>
-      </c>
-      <c r="V32" s="3" t="s">
+      <c r="V32" t="s">
+        <v>59</v>
+      </c>
+      <c r="W32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W32" s="3" t="s">
+      <c r="X32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="X32" s="11"/>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <v>45181</v>
       </c>
@@ -3066,54 +3169,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F33" t="s">
-        <v>0</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="F33" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I33" t="s">
         <v>0</v>
       </c>
-      <c r="J33" t="str">
+      <c r="J33" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K33" t="s">
-        <v>101</v>
-      </c>
-      <c r="L33">
+      <c r="L33" t="s">
+        <v>100</v>
+      </c>
+      <c r="M33">
         <v>6</v>
       </c>
-      <c r="M33" s="8">
-        <f t="shared" si="4"/>
+      <c r="N33" s="8">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="R33" t="s">
-        <v>0</v>
-      </c>
       <c r="S33" t="s">
         <v>0</v>
       </c>
-      <c r="T33" s="8">
+      <c r="T33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U33" s="8">
         <f t="shared" si="7"/>
         <v>22533</v>
       </c>
-      <c r="U33" t="s">
-        <v>77</v>
-      </c>
-      <c r="V33" s="3" t="s">
+      <c r="V33" t="s">
+        <v>76</v>
+      </c>
+      <c r="W33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="W33" s="3" t="s">
+      <c r="X33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X33" s="11"/>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <v>45188</v>
       </c>
@@ -3131,54 +3236,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F34" t="s">
-        <v>0</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="F34" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I34" t="s">
         <v>0</v>
       </c>
-      <c r="J34" t="str">
+      <c r="J34" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K34" t="s">
-        <v>101</v>
-      </c>
-      <c r="L34">
+      <c r="L34" t="s">
+        <v>100</v>
+      </c>
+      <c r="M34">
         <v>5</v>
       </c>
-      <c r="M34" s="8">
-        <f t="shared" si="4"/>
+      <c r="N34" s="8">
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="R34" t="s">
-        <v>0</v>
-      </c>
       <c r="S34" t="s">
         <v>0</v>
       </c>
-      <c r="T34" s="8">
+      <c r="T34" t="s">
+        <v>0</v>
+      </c>
+      <c r="U34" s="8">
         <f t="shared" si="7"/>
         <v>22568</v>
       </c>
-      <c r="U34" t="s">
-        <v>60</v>
-      </c>
-      <c r="V34" s="3" t="s">
+      <c r="V34" t="s">
+        <v>59</v>
+      </c>
+      <c r="W34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="W34" s="3" t="s">
+      <c r="X34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X34" s="11"/>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
         <v>45195</v>
       </c>
@@ -3196,54 +3303,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F35" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="F35" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I35" t="s">
         <v>0</v>
       </c>
-      <c r="J35" t="str">
+      <c r="J35" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K35" t="s">
-        <v>102</v>
-      </c>
-      <c r="L35">
+      <c r="L35" t="s">
+        <v>101</v>
+      </c>
+      <c r="M35">
         <v>4</v>
       </c>
-      <c r="M35" s="8">
-        <f t="shared" si="4"/>
+      <c r="N35" s="8">
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="R35" t="s">
-        <v>0</v>
-      </c>
       <c r="S35" t="s">
         <v>0</v>
       </c>
-      <c r="T35" s="8">
+      <c r="T35" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="8">
         <f t="shared" si="7"/>
         <v>22596</v>
       </c>
-      <c r="U35" t="s">
-        <v>67</v>
-      </c>
-      <c r="V35" s="3" t="s">
+      <c r="V35" t="s">
+        <v>66</v>
+      </c>
+      <c r="W35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W35" s="3" t="s">
+      <c r="X35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X35" s="11"/>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>45202</v>
       </c>
@@ -3261,54 +3370,56 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F36" t="s">
-        <v>0</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="F36" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I36" t="s">
         <v>0</v>
       </c>
-      <c r="J36" t="str">
+      <c r="J36" t="s">
+        <v>0</v>
+      </c>
+      <c r="K36" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K36" t="s">
-        <v>64</v>
-      </c>
-      <c r="L36">
+      <c r="L36" t="s">
+        <v>63</v>
+      </c>
+      <c r="M36">
         <v>3</v>
       </c>
-      <c r="M36" s="8">
-        <f t="shared" si="4"/>
+      <c r="N36" s="8">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="R36" t="s">
-        <v>0</v>
-      </c>
       <c r="S36" t="s">
         <v>0</v>
       </c>
-      <c r="T36" s="8">
+      <c r="T36" t="s">
+        <v>0</v>
+      </c>
+      <c r="U36" s="8">
         <f t="shared" si="7"/>
         <v>22617</v>
       </c>
-      <c r="U36" t="s">
-        <v>67</v>
-      </c>
-      <c r="V36" s="3" t="s">
+      <c r="V36" t="s">
+        <v>66</v>
+      </c>
+      <c r="W36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="W36" s="3" t="s">
+      <c r="X36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="X36" s="11"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="13">
         <v>45209</v>
       </c>
@@ -3326,122 +3437,193 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F37" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="F37" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I37" t="s">
         <v>0</v>
       </c>
-      <c r="J37" t="str">
+      <c r="J37" t="s">
+        <v>0</v>
+      </c>
+      <c r="K37" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="K37" t="s">
-        <v>75</v>
-      </c>
-      <c r="L37">
+      <c r="L37" t="s">
+        <v>74</v>
+      </c>
+      <c r="M37">
         <v>6</v>
       </c>
-      <c r="M37" s="8">
-        <f t="shared" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="R37" t="s">
-        <v>0</v>
+      <c r="N37" s="11">
+        <v>44</v>
       </c>
       <c r="S37" t="s">
         <v>0</v>
       </c>
-      <c r="T37" s="8">
-        <f t="shared" si="7"/>
-        <v>22659</v>
-      </c>
-      <c r="U37" t="s">
-        <v>64</v>
-      </c>
-      <c r="V37" s="3" t="s">
+      <c r="T37" t="s">
+        <v>0</v>
+      </c>
+      <c r="U37" s="8">
+        <f>U36+N37</f>
+        <v>22661</v>
+      </c>
+      <c r="V37" t="s">
+        <v>63</v>
+      </c>
+      <c r="W37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="W37" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="X37" s="11" t="s">
-        <v>35</v>
+      <c r="X37" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y37" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" s="13">
+        <v>45216</v>
+      </c>
+      <c r="B38" s="13">
+        <v>45222</v>
+      </c>
+      <c r="C38" s="13">
+        <f>B38</f>
+        <v>45222</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" ref="K38" si="13">I38</f>
+        <v>NA</v>
+      </c>
+      <c r="L38" t="s">
+        <v>100</v>
+      </c>
+      <c r="M38" t="s">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>29</v>
+      </c>
+      <c r="S38" t="s">
+        <v>0</v>
+      </c>
+      <c r="T38" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="8">
+        <f>U37+N38</f>
+        <v>22690</v>
+      </c>
+      <c r="V38" t="s">
+        <v>100</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y38" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V37" r:id="rId1" xr:uid="{59A81795-EA5B-AA48-B26A-7020BAA2B369}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{561DF127-44C1-0F4B-B09F-F91BFBB25223}"/>
-    <hyperlink ref="V3" r:id="rId3" xr:uid="{A5D4D65C-1F39-4248-BC71-A74182399E5A}"/>
-    <hyperlink ref="V4" r:id="rId4" xr:uid="{610C6DF1-7DF5-D148-B367-D12AFF761ADD}"/>
-    <hyperlink ref="V5" r:id="rId5" xr:uid="{0CC70FA3-D6AB-9A41-87B4-2BEEE7140FE1}"/>
-    <hyperlink ref="V6" r:id="rId6" xr:uid="{CD2FE2AB-A1C6-9542-840F-D06E9D54EC1F}"/>
-    <hyperlink ref="V7" r:id="rId7" xr:uid="{C4F3CF49-03F3-5D40-88A3-EF4CCF4C1D9C}"/>
-    <hyperlink ref="V9" r:id="rId8" xr:uid="{0EE8C3D6-3F3C-4843-B844-F6AB8565DA70}"/>
-    <hyperlink ref="V10" r:id="rId9" xr:uid="{C2CAB875-494C-FC4B-B0BE-87C053DE6D2D}"/>
-    <hyperlink ref="V16" r:id="rId10" xr:uid="{DA0AA8D6-E80D-244C-A700-12E9EDBD7513}"/>
-    <hyperlink ref="V17" r:id="rId11" xr:uid="{E0113175-6B3F-7E42-B9DA-5B05785C0B27}"/>
-    <hyperlink ref="V18" r:id="rId12" xr:uid="{6B944ACD-8D2C-DC49-9D48-A0F819EF9F5F}"/>
-    <hyperlink ref="V13" r:id="rId13" xr:uid="{7B952E61-8544-3644-87FD-03C2920F7729}"/>
-    <hyperlink ref="V14" r:id="rId14" xr:uid="{D74CE0DB-60F2-F241-BC21-34FB7076A183}"/>
-    <hyperlink ref="V15" r:id="rId15" xr:uid="{F3AA72B2-E388-7546-AA91-815C1F4067A7}"/>
-    <hyperlink ref="V20" r:id="rId16" xr:uid="{AB47D2A9-57CE-644B-B903-576151BAAE2A}"/>
-    <hyperlink ref="V21" r:id="rId17" xr:uid="{0DE1C71B-AA16-9345-B13E-8E1EDC80148A}"/>
-    <hyperlink ref="V22" r:id="rId18" xr:uid="{F604421D-990C-4D40-B64E-321E72471444}"/>
-    <hyperlink ref="V23" r:id="rId19" xr:uid="{DF600EA1-218D-F140-A264-5F1C6421FA3A}"/>
-    <hyperlink ref="V24" r:id="rId20" xr:uid="{1E137D19-E456-1241-B6B8-12CECCC2A53D}"/>
-    <hyperlink ref="V25" r:id="rId21" xr:uid="{59543A3C-AC8C-0F41-A052-EF53E1D01F77}"/>
-    <hyperlink ref="V26" r:id="rId22" xr:uid="{403A442F-6C9B-DF4C-8C5C-DD9F6C3188CD}"/>
-    <hyperlink ref="V27" r:id="rId23" xr:uid="{66B5E2CF-E5E2-EC42-B7BF-A56E58EA5C22}"/>
-    <hyperlink ref="V28" r:id="rId24" xr:uid="{C925BA72-B753-1B44-B269-89BB6BAB76D4}"/>
-    <hyperlink ref="V30" r:id="rId25" xr:uid="{A83290C0-5AFC-0E4A-9A46-8CE2ADC9A489}"/>
-    <hyperlink ref="V31" r:id="rId26" xr:uid="{AF25C658-5256-9E4E-8F67-AF94603EA12F}"/>
-    <hyperlink ref="V32" r:id="rId27" xr:uid="{9AD1292C-491B-314E-8C1D-05E74041B5F1}"/>
-    <hyperlink ref="V33" r:id="rId28" xr:uid="{2F102B49-2FC8-524E-9B76-E7CD46B22189}"/>
-    <hyperlink ref="V34" r:id="rId29" xr:uid="{64E8491F-C3F2-9E46-A259-601E2C41D26B}"/>
-    <hyperlink ref="V35" r:id="rId30" xr:uid="{BB5B84AB-6F7B-B244-A174-1A512535795C}"/>
-    <hyperlink ref="V36" r:id="rId31" xr:uid="{8870BAAB-A73B-3C48-94DA-CA93FDE0B85F}"/>
-    <hyperlink ref="W5" r:id="rId32" xr:uid="{2909190A-C9EE-FD43-8645-3FCC15B58166}"/>
-    <hyperlink ref="W6" r:id="rId33" xr:uid="{974F0896-592F-2F42-BB67-974FF4B85C6C}"/>
-    <hyperlink ref="V8" r:id="rId34" xr:uid="{7E1E41CE-39EC-C345-89EA-98A620EF3493}"/>
-    <hyperlink ref="W7" r:id="rId35" xr:uid="{C05DE0B7-FD85-724C-9F04-33C2071064DA}"/>
-    <hyperlink ref="W8" r:id="rId36" xr:uid="{52B18004-C3C9-0F4F-B7E1-E6DFD43880B2}"/>
-    <hyperlink ref="W9" r:id="rId37" xr:uid="{1E04F05A-18A6-F149-AB3E-EAB03CFD7421}"/>
-    <hyperlink ref="V11" r:id="rId38" xr:uid="{B1F2917E-F280-2649-B418-77AA63C5C46B}"/>
-    <hyperlink ref="W10" r:id="rId39" xr:uid="{22B2FBC5-A2A0-4F42-B6F2-B1368A268DB5}"/>
-    <hyperlink ref="V12" r:id="rId40" xr:uid="{D2EACEB9-88B1-5B4C-8698-51818D5808DC}"/>
-    <hyperlink ref="W12" r:id="rId41" xr:uid="{6C5F8229-489C-CE44-AF4E-9F6785A9CEBA}"/>
-    <hyperlink ref="W13" r:id="rId42" xr:uid="{93B942DA-5304-C14A-8E2A-BD96AD5308D0}"/>
-    <hyperlink ref="W11" r:id="rId43" xr:uid="{916CDA71-6EA6-864F-8A1D-9B08126D77A4}"/>
-    <hyperlink ref="W14" r:id="rId44" xr:uid="{9BFFF453-0041-FD4A-82B4-014558B1E79C}"/>
-    <hyperlink ref="W15" r:id="rId45" xr:uid="{70784B18-A29D-954F-B393-2DBB163032D4}"/>
-    <hyperlink ref="W16" r:id="rId46" xr:uid="{D695395C-92F6-774A-B0E2-2D7F066DF0FD}"/>
-    <hyperlink ref="W17" r:id="rId47" xr:uid="{AF74BD6D-13FE-2746-BB55-99B057D26EE0}"/>
-    <hyperlink ref="V19" r:id="rId48" xr:uid="{C3B1E930-E323-634B-BCDE-49FF8812A9A5}"/>
-    <hyperlink ref="W18" r:id="rId49" xr:uid="{B814BEF3-8A73-5A4C-AD98-D087B165E3EE}"/>
-    <hyperlink ref="W19" r:id="rId50" xr:uid="{13F64D78-43F7-1648-B3E4-E740E707B6DC}"/>
-    <hyperlink ref="W20" r:id="rId51" xr:uid="{F0FAC90B-C022-1E41-8EC4-A5FDB868E462}"/>
-    <hyperlink ref="W21" r:id="rId52" xr:uid="{55CA12C2-537E-314A-9E36-EC3DFF4BF6C7}"/>
-    <hyperlink ref="W22" r:id="rId53" xr:uid="{3EC451B3-9FA4-A343-96CD-0389AADB6D41}"/>
-    <hyperlink ref="W23" r:id="rId54" xr:uid="{A4810EA8-338C-894E-98E7-463A9C146FE0}"/>
-    <hyperlink ref="W24" r:id="rId55" xr:uid="{5A308C05-B2A5-3E4F-96AB-C0FF5235F44A}"/>
-    <hyperlink ref="W25" r:id="rId56" xr:uid="{82E3C59F-7571-D34C-AF4D-0EF4BDD7F52D}"/>
-    <hyperlink ref="W26" r:id="rId57" xr:uid="{C23F1784-0828-1649-9EFB-D78079DCFCF1}"/>
-    <hyperlink ref="W27" r:id="rId58" xr:uid="{911824AA-2747-A34F-8F0C-12918F5F03C0}"/>
-    <hyperlink ref="W30" r:id="rId59" xr:uid="{7C9C018A-FDF2-484C-85F6-4B6DE2D95EBF}"/>
-    <hyperlink ref="W31" r:id="rId60" xr:uid="{4590BFEB-27E8-8949-ADE8-70E4E255C8AB}"/>
-    <hyperlink ref="W32" r:id="rId61" xr:uid="{493943D6-667F-B44B-A12B-2DA09EC6CE7A}"/>
-    <hyperlink ref="W33" r:id="rId62" xr:uid="{36E74884-1DCF-1548-82C2-83224C0494BD}"/>
-    <hyperlink ref="W34" r:id="rId63" xr:uid="{B19EA63D-01E7-D44C-934F-6D3FA7D10EA1}"/>
-    <hyperlink ref="W35" r:id="rId64" xr:uid="{BBBF4FD9-0337-9E42-97FA-04332AC66CF6}"/>
-    <hyperlink ref="W36" r:id="rId65" xr:uid="{FF4BFBC6-CABC-E742-9D2A-4C479C18B7A7}"/>
+    <hyperlink ref="W37" r:id="rId1" xr:uid="{59A81795-EA5B-AA48-B26A-7020BAA2B369}"/>
+    <hyperlink ref="W2" r:id="rId2" xr:uid="{561DF127-44C1-0F4B-B09F-F91BFBB25223}"/>
+    <hyperlink ref="W3" r:id="rId3" xr:uid="{A5D4D65C-1F39-4248-BC71-A74182399E5A}"/>
+    <hyperlink ref="W4" r:id="rId4" xr:uid="{610C6DF1-7DF5-D148-B367-D12AFF761ADD}"/>
+    <hyperlink ref="W5" r:id="rId5" xr:uid="{0CC70FA3-D6AB-9A41-87B4-2BEEE7140FE1}"/>
+    <hyperlink ref="W6" r:id="rId6" xr:uid="{CD2FE2AB-A1C6-9542-840F-D06E9D54EC1F}"/>
+    <hyperlink ref="W7" r:id="rId7" xr:uid="{C4F3CF49-03F3-5D40-88A3-EF4CCF4C1D9C}"/>
+    <hyperlink ref="W9" r:id="rId8" xr:uid="{0EE8C3D6-3F3C-4843-B844-F6AB8565DA70}"/>
+    <hyperlink ref="W10" r:id="rId9" xr:uid="{C2CAB875-494C-FC4B-B0BE-87C053DE6D2D}"/>
+    <hyperlink ref="W16" r:id="rId10" xr:uid="{DA0AA8D6-E80D-244C-A700-12E9EDBD7513}"/>
+    <hyperlink ref="W17" r:id="rId11" xr:uid="{E0113175-6B3F-7E42-B9DA-5B05785C0B27}"/>
+    <hyperlink ref="W18" r:id="rId12" xr:uid="{6B944ACD-8D2C-DC49-9D48-A0F819EF9F5F}"/>
+    <hyperlink ref="W13" r:id="rId13" xr:uid="{7B952E61-8544-3644-87FD-03C2920F7729}"/>
+    <hyperlink ref="W14" r:id="rId14" xr:uid="{D74CE0DB-60F2-F241-BC21-34FB7076A183}"/>
+    <hyperlink ref="W15" r:id="rId15" xr:uid="{F3AA72B2-E388-7546-AA91-815C1F4067A7}"/>
+    <hyperlink ref="W20" r:id="rId16" xr:uid="{AB47D2A9-57CE-644B-B903-576151BAAE2A}"/>
+    <hyperlink ref="W21" r:id="rId17" xr:uid="{0DE1C71B-AA16-9345-B13E-8E1EDC80148A}"/>
+    <hyperlink ref="W22" r:id="rId18" xr:uid="{F604421D-990C-4D40-B64E-321E72471444}"/>
+    <hyperlink ref="W23" r:id="rId19" xr:uid="{DF600EA1-218D-F140-A264-5F1C6421FA3A}"/>
+    <hyperlink ref="W24" r:id="rId20" xr:uid="{1E137D19-E456-1241-B6B8-12CECCC2A53D}"/>
+    <hyperlink ref="W25" r:id="rId21" xr:uid="{59543A3C-AC8C-0F41-A052-EF53E1D01F77}"/>
+    <hyperlink ref="W26" r:id="rId22" xr:uid="{403A442F-6C9B-DF4C-8C5C-DD9F6C3188CD}"/>
+    <hyperlink ref="W27" r:id="rId23" xr:uid="{66B5E2CF-E5E2-EC42-B7BF-A56E58EA5C22}"/>
+    <hyperlink ref="W28" r:id="rId24" xr:uid="{C925BA72-B753-1B44-B269-89BB6BAB76D4}"/>
+    <hyperlink ref="W30" r:id="rId25" xr:uid="{A83290C0-5AFC-0E4A-9A46-8CE2ADC9A489}"/>
+    <hyperlink ref="W31" r:id="rId26" xr:uid="{AF25C658-5256-9E4E-8F67-AF94603EA12F}"/>
+    <hyperlink ref="W32" r:id="rId27" xr:uid="{9AD1292C-491B-314E-8C1D-05E74041B5F1}"/>
+    <hyperlink ref="W33" r:id="rId28" xr:uid="{2F102B49-2FC8-524E-9B76-E7CD46B22189}"/>
+    <hyperlink ref="W34" r:id="rId29" xr:uid="{64E8491F-C3F2-9E46-A259-601E2C41D26B}"/>
+    <hyperlink ref="W35" r:id="rId30" xr:uid="{BB5B84AB-6F7B-B244-A174-1A512535795C}"/>
+    <hyperlink ref="W36" r:id="rId31" xr:uid="{8870BAAB-A73B-3C48-94DA-CA93FDE0B85F}"/>
+    <hyperlink ref="X5" r:id="rId32" xr:uid="{2909190A-C9EE-FD43-8645-3FCC15B58166}"/>
+    <hyperlink ref="X6" r:id="rId33" xr:uid="{974F0896-592F-2F42-BB67-974FF4B85C6C}"/>
+    <hyperlink ref="W8" r:id="rId34" xr:uid="{7E1E41CE-39EC-C345-89EA-98A620EF3493}"/>
+    <hyperlink ref="X7" r:id="rId35" xr:uid="{C05DE0B7-FD85-724C-9F04-33C2071064DA}"/>
+    <hyperlink ref="X8" r:id="rId36" xr:uid="{52B18004-C3C9-0F4F-B7E1-E6DFD43880B2}"/>
+    <hyperlink ref="X9" r:id="rId37" xr:uid="{1E04F05A-18A6-F149-AB3E-EAB03CFD7421}"/>
+    <hyperlink ref="W11" r:id="rId38" xr:uid="{B1F2917E-F280-2649-B418-77AA63C5C46B}"/>
+    <hyperlink ref="X10" r:id="rId39" xr:uid="{22B2FBC5-A2A0-4F42-B6F2-B1368A268DB5}"/>
+    <hyperlink ref="W12" r:id="rId40" xr:uid="{D2EACEB9-88B1-5B4C-8698-51818D5808DC}"/>
+    <hyperlink ref="X12" r:id="rId41" xr:uid="{6C5F8229-489C-CE44-AF4E-9F6785A9CEBA}"/>
+    <hyperlink ref="X13" r:id="rId42" xr:uid="{93B942DA-5304-C14A-8E2A-BD96AD5308D0}"/>
+    <hyperlink ref="X11" r:id="rId43" xr:uid="{916CDA71-6EA6-864F-8A1D-9B08126D77A4}"/>
+    <hyperlink ref="X14" r:id="rId44" xr:uid="{9BFFF453-0041-FD4A-82B4-014558B1E79C}"/>
+    <hyperlink ref="X15" r:id="rId45" xr:uid="{70784B18-A29D-954F-B393-2DBB163032D4}"/>
+    <hyperlink ref="X16" r:id="rId46" xr:uid="{D695395C-92F6-774A-B0E2-2D7F066DF0FD}"/>
+    <hyperlink ref="X17" r:id="rId47" xr:uid="{AF74BD6D-13FE-2746-BB55-99B057D26EE0}"/>
+    <hyperlink ref="W19" r:id="rId48" xr:uid="{C3B1E930-E323-634B-BCDE-49FF8812A9A5}"/>
+    <hyperlink ref="X18" r:id="rId49" xr:uid="{B814BEF3-8A73-5A4C-AD98-D087B165E3EE}"/>
+    <hyperlink ref="X19" r:id="rId50" xr:uid="{13F64D78-43F7-1648-B3E4-E740E707B6DC}"/>
+    <hyperlink ref="X20" r:id="rId51" xr:uid="{F0FAC90B-C022-1E41-8EC4-A5FDB868E462}"/>
+    <hyperlink ref="X21" r:id="rId52" xr:uid="{55CA12C2-537E-314A-9E36-EC3DFF4BF6C7}"/>
+    <hyperlink ref="X22" r:id="rId53" xr:uid="{3EC451B3-9FA4-A343-96CD-0389AADB6D41}"/>
+    <hyperlink ref="X23" r:id="rId54" xr:uid="{A4810EA8-338C-894E-98E7-463A9C146FE0}"/>
+    <hyperlink ref="X24" r:id="rId55" xr:uid="{5A308C05-B2A5-3E4F-96AB-C0FF5235F44A}"/>
+    <hyperlink ref="X25" r:id="rId56" xr:uid="{82E3C59F-7571-D34C-AF4D-0EF4BDD7F52D}"/>
+    <hyperlink ref="X26" r:id="rId57" xr:uid="{C23F1784-0828-1649-9EFB-D78079DCFCF1}"/>
+    <hyperlink ref="X27" r:id="rId58" xr:uid="{911824AA-2747-A34F-8F0C-12918F5F03C0}"/>
+    <hyperlink ref="X30" r:id="rId59" xr:uid="{7C9C018A-FDF2-484C-85F6-4B6DE2D95EBF}"/>
+    <hyperlink ref="X31" r:id="rId60" xr:uid="{4590BFEB-27E8-8949-ADE8-70E4E255C8AB}"/>
+    <hyperlink ref="X32" r:id="rId61" xr:uid="{493943D6-667F-B44B-A12B-2DA09EC6CE7A}"/>
+    <hyperlink ref="X33" r:id="rId62" xr:uid="{36E74884-1DCF-1548-82C2-83224C0494BD}"/>
+    <hyperlink ref="X34" r:id="rId63" xr:uid="{B19EA63D-01E7-D44C-934F-6D3FA7D10EA1}"/>
+    <hyperlink ref="X35" r:id="rId64" xr:uid="{BBBF4FD9-0337-9E42-97FA-04332AC66CF6}"/>
+    <hyperlink ref="X36" r:id="rId65" xr:uid="{FF4BFBC6-CABC-E742-9D2A-4C479C18B7A7}"/>
+    <hyperlink ref="X37" r:id="rId66" xr:uid="{62C459D7-F921-AC4A-862F-335EF0E8D904}"/>
+    <hyperlink ref="W38" r:id="rId67" xr:uid="{F1C37EFA-2085-8646-80D1-89A443C6D10A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update for Taiwan CDC data release on 20231031
</commit_message>
<xml_diff>
--- a/Taiwan-COVID19-data-2023.xlsx
+++ b/Taiwan-COVID19-data-2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chasenelson/scripts_NGS/github_Taiwan-COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119165F0-39E5-EB4E-8833-D25B8C8AAA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1584544F-7B9C-A248-80FE-7E70901D38EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{836FDAF7-E370-6E4C-85E6-CE82AA0CAB02}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="116">
   <si>
     <t>NA</t>
   </si>
@@ -374,7 +374,16 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Taiwan CDC changed its reporting, evidently in response to this repository posting on 20231023; new_deaths is now reported explicitly; DATES are not given</t>
+    <t>"slightly lower"</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/VY3ZmLYRFjSOAuJmCF9K2g?typeid=9</t>
+  </si>
+  <si>
+    <t>Last week's DATES are no longer given</t>
+  </si>
+  <si>
+    <t>Taiwan CDC changed its reporting, evidently in response to this repository posting on 20231023; new_deaths is now reported explicitly; last week's DATES are not given</t>
   </si>
 </sst>
 </file>
@@ -848,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4771C105-BA87-EE45-8165-DB3BB9CF7A30}">
-  <dimension ref="A1:Y38"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -969,7 +978,7 @@
         <v>44980</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D38" si="0">B2-A2+1</f>
+        <f t="shared" ref="D2:D39" si="0">B2-A2+1</f>
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1053,7 +1062,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E38" si="2">A3-B2-1</f>
+        <f t="shared" ref="E3:E39" si="2">A3-B2-1</f>
         <v>0</v>
       </c>
       <c r="F3" s="19" t="s">
@@ -3551,8 +3560,81 @@
       <c r="W38" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="X38" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="Y38" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
+        <v>45223</v>
+      </c>
+      <c r="B39" s="13">
+        <v>45229</v>
+      </c>
+      <c r="C39" s="13">
+        <f>B39</f>
+        <v>45229</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" ref="K39" si="14">I39</f>
+        <v>NA</v>
+      </c>
+      <c r="L39" t="s">
         <v>112</v>
+      </c>
+      <c r="M39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>35</v>
+      </c>
+      <c r="S39" t="s">
+        <v>0</v>
+      </c>
+      <c r="T39" t="s">
+        <v>0</v>
+      </c>
+      <c r="U39" s="8">
+        <f>U38+N39</f>
+        <v>22725</v>
+      </c>
+      <c r="V39" t="s">
+        <v>71</v>
+      </c>
+      <c r="W39" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="X39" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3624,7 +3706,10 @@
     <hyperlink ref="X36" r:id="rId65" xr:uid="{FF4BFBC6-CABC-E742-9D2A-4C479C18B7A7}"/>
     <hyperlink ref="X37" r:id="rId66" xr:uid="{62C459D7-F921-AC4A-862F-335EF0E8D904}"/>
     <hyperlink ref="W38" r:id="rId67" xr:uid="{F1C37EFA-2085-8646-80D1-89A443C6D10A}"/>
+    <hyperlink ref="W39" r:id="rId68" xr:uid="{A7F628F0-78D8-3344-B07D-61EF645F5803}"/>
+    <hyperlink ref="X38" r:id="rId69" xr:uid="{00B64168-1F56-BB49-8FFB-7073B35C4751}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for Taiwan CDC data release on 20231121
</commit_message>
<xml_diff>
--- a/Taiwan-COVID19-data-2023.xlsx
+++ b/Taiwan-COVID19-data-2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chasenelson/scripts_NGS/github_Taiwan-COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1584544F-7B9C-A248-80FE-7E70901D38EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA316E52-56AB-9646-AF98-E6AE95446062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{836FDAF7-E370-6E4C-85E6-CE82AA0CAB02}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="120">
   <si>
     <t>NA</t>
   </si>
@@ -384,6 +384,18 @@
   </si>
   <si>
     <t>Taiwan CDC changed its reporting, evidently in response to this repository posting on 20231023; new_deaths is now reported explicitly; last week's DATES are not given</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Ak-qBnA0516o81THvVZEoA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/tIvtKfKPGYMiHMK8BGyqXQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/nu5ANEWfikBAebIZ6_7mDg?typeid=9</t>
+  </si>
+  <si>
+    <t>DATES are now given again, presumably at my (unanswered) request</t>
   </si>
 </sst>
 </file>
@@ -857,10 +869,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4771C105-BA87-EE45-8165-DB3BB9CF7A30}">
-  <dimension ref="A1:Y39"/>
+  <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A1:Y42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3630,11 +3643,218 @@
       <c r="W39" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="X39" s="7" t="s">
-        <v>0</v>
+      <c r="X39" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="Y39" s="11" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" s="13">
+        <v>45230</v>
+      </c>
+      <c r="B40" s="13">
+        <v>45236</v>
+      </c>
+      <c r="C40" s="13">
+        <f t="shared" ref="C40:C42" si="15">B40</f>
+        <v>45236</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" ref="D40:D42" si="16">B40-A40+1</f>
+        <v>7</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" ref="E40:E42" si="17">A40-B39-1</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G40" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>0</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" ref="K40" si="18">I40</f>
+        <v>NA</v>
+      </c>
+      <c r="L40" t="s">
+        <v>100</v>
+      </c>
+      <c r="M40" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>28</v>
+      </c>
+      <c r="S40" t="s">
+        <v>0</v>
+      </c>
+      <c r="T40" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="8">
+        <f t="shared" ref="U40:U42" si="19">U39+N40</f>
+        <v>22753</v>
+      </c>
+      <c r="V40" t="s">
+        <v>100</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y40" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A41" s="13">
+        <v>45237</v>
+      </c>
+      <c r="B41" s="13">
+        <v>45243</v>
+      </c>
+      <c r="C41" s="13">
+        <f t="shared" si="15"/>
+        <v>45243</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>0</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" ref="K41" si="20">I41</f>
+        <v>NA</v>
+      </c>
+      <c r="L41" t="s">
+        <v>74</v>
+      </c>
+      <c r="M41" t="s">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>29</v>
+      </c>
+      <c r="S41" t="s">
+        <v>0</v>
+      </c>
+      <c r="T41" t="s">
+        <v>0</v>
+      </c>
+      <c r="U41" s="8">
+        <f t="shared" si="19"/>
+        <v>22782</v>
+      </c>
+      <c r="V41" t="s">
+        <v>69</v>
+      </c>
+      <c r="W41" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="X41" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y41" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42" s="13">
+        <v>45244</v>
+      </c>
+      <c r="B42" s="13">
+        <v>45250</v>
+      </c>
+      <c r="C42" s="13">
+        <f t="shared" si="15"/>
+        <v>45250</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>0</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" ref="K42" si="21">I42</f>
+        <v>NA</v>
+      </c>
+      <c r="L42" t="s">
+        <v>100</v>
+      </c>
+      <c r="M42" t="s">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>24</v>
+      </c>
+      <c r="S42" t="s">
+        <v>0</v>
+      </c>
+      <c r="T42" t="s">
+        <v>0</v>
+      </c>
+      <c r="U42" s="8">
+        <f t="shared" si="19"/>
+        <v>22806</v>
+      </c>
+      <c r="V42" t="s">
+        <v>100</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="X42" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3708,6 +3928,12 @@
     <hyperlink ref="W38" r:id="rId67" xr:uid="{F1C37EFA-2085-8646-80D1-89A443C6D10A}"/>
     <hyperlink ref="W39" r:id="rId68" xr:uid="{A7F628F0-78D8-3344-B07D-61EF645F5803}"/>
     <hyperlink ref="X38" r:id="rId69" xr:uid="{00B64168-1F56-BB49-8FFB-7073B35C4751}"/>
+    <hyperlink ref="W42" r:id="rId70" xr:uid="{7432B6EB-A946-7F4B-8DD8-FDE1D8B8BAA2}"/>
+    <hyperlink ref="X41" r:id="rId71" xr:uid="{25A82B89-E585-794E-8F08-57D377A7D6A5}"/>
+    <hyperlink ref="W41" r:id="rId72" xr:uid="{9FD58D5E-0DB3-CF43-9444-5D62003CD7AD}"/>
+    <hyperlink ref="X40" r:id="rId73" xr:uid="{E3339B81-D73F-8444-A9E9-DF4DA5C47308}"/>
+    <hyperlink ref="X39" r:id="rId74" xr:uid="{BFDB6758-74B4-714D-A7E9-8F3A1E917896}"/>
+    <hyperlink ref="W40" r:id="rId75" xr:uid="{D1D85DA0-EB5B-864B-9759-40CF52B4E042}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>